<commit_message>
release PMIR 1.5.0 for TI
</commit_message>
<xml_diff>
--- a/ITI/PMIR/StructureDefinition-IHE.PMIR.Audit.Subscription.Create.xlsx
+++ b/ITI/PMIR/StructureDefinition-IHE.PMIR.Audit.Subscription.Create.xlsx
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.4.0</t>
+    <t>1.5.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-05-12T07:36:47-05:00</t>
+    <t>2022-08-08T16:08:06-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -2212,7 +2212,7 @@
     <col min="1" max="1" width="41.4609375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="11.15234375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="5.90234375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="5.07421875" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="14.625" customWidth="true" bestFit="true"/>
@@ -2228,28 +2228,28 @@
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="15.7109375" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="16.0859375" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="15.71484375" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="16.08984375" customWidth="true" bestFit="true"/>
     <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="16.3125" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="95.56640625" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="54.15625" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="14.984375" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="12.30078125" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="40.0390625" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="14.98828125" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="12.3046875" customWidth="true" bestFit="true"/>
     <col min="31" max="31" width="34.0703125" customWidth="true" bestFit="true" hidden="true"/>
     <col min="32" max="32" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="9.87890625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="34" max="34" width="12.21875" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="36" max="36" width="26.71484375" customWidth="true" bestFit="true"/>
+    <col min="36" max="36" width="26.71875" customWidth="true" bestFit="true"/>
     <col min="37" max="37" width="155.37890625" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="49.38671875" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="49.390625" customWidth="true" bestFit="true"/>
     <col min="39" max="39" width="32.84375" customWidth="true" bestFit="true"/>
     <col min="40" max="40" width="34.4140625" customWidth="true" bestFit="true"/>
-    <col min="41" max="41" width="40.0" customWidth="true" bestFit="true"/>
+    <col min="41" max="41" width="40.00390625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>